<commit_message>
update task list by vmcuong
</commit_message>
<xml_diff>
--- a/Task list.xlsx
+++ b/Task list.xlsx
@@ -104,7 +104,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -302,13 +302,13 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -665,7 +665,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="28.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="27.75" customFormat="1" s="1">
       <c r="A2" s="10" t="s">
         <v>9</v>
       </c>
@@ -695,15 +695,15 @@
       </c>
       <c r="J2" s="15"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="62.25" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="33.75" customFormat="1" s="1">
       <c r="A3" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="17">
-        <v>44653</v>
-      </c>
-      <c r="C3" s="17">
-        <v>44655</v>
+      <c r="B3" s="11">
+        <v>44656</v>
+      </c>
+      <c r="C3" s="11">
+        <v>44656</v>
       </c>
       <c r="D3" s="14">
         <v>1</v>

</xml_diff>